<commit_message>
create test case sign up
</commit_message>
<xml_diff>
--- a/com.apartments/src/test/resources/test_data.xlsx
+++ b/com.apartments/src/test/resources/test_data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>email</t>
   </si>
@@ -25,24 +25,12 @@
     <t>password</t>
   </si>
   <si>
-    <t>abc1@gmail.com</t>
-  </si>
-  <si>
-    <t>AydenLiam1213</t>
-  </si>
-  <si>
     <t>toubouachefazia@gmail.com</t>
   </si>
   <si>
     <t>Fazia@96us</t>
   </si>
   <si>
-    <t>abctestemail2378!!!!@gmail.com</t>
-  </si>
-  <si>
-    <t>QqwertyQ@123!</t>
-  </si>
-  <si>
     <t>phoneNumber</t>
   </si>
   <si>
@@ -55,18 +43,9 @@
     <t>223-334-5589</t>
   </si>
   <si>
-    <t>carmel</t>
-  </si>
-  <si>
     <t>westfield</t>
   </si>
   <si>
-    <t>noblesville</t>
-  </si>
-  <si>
-    <t>fishers</t>
-  </si>
-  <si>
     <t>209-998-7765</t>
   </si>
   <si>
@@ -83,6 +62,45 @@
   </si>
   <si>
     <t>916-657-4576</t>
+  </si>
+  <si>
+    <t>fazousara96@yahoo.com</t>
+  </si>
+  <si>
+    <t>Abc1996@us</t>
+  </si>
+  <si>
+    <t>fazousaradouni@gmail.com</t>
+  </si>
+  <si>
+    <t>Fabc1996@us</t>
+  </si>
+  <si>
+    <t>SearchTerm</t>
+  </si>
+  <si>
+    <t>1235 IN, Carmel</t>
+  </si>
+  <si>
+    <t>1277 IN, Westfield</t>
+  </si>
+  <si>
+    <t>46074 IN, Westfield</t>
+  </si>
+  <si>
+    <t>46240 IN, Nora</t>
+  </si>
+  <si>
+    <t>46069 IN,Sheridan</t>
+  </si>
+  <si>
+    <t>Carmel</t>
+  </si>
+  <si>
+    <t>Noblesville</t>
+  </si>
+  <si>
+    <t>Fishers</t>
   </si>
 </sst>
 </file>
@@ -427,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -448,26 +466,36 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
     <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="B4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -475,10 +503,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -498,13 +526,34 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="B4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -515,7 +564,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -526,57 +575,57 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -586,12 +635,45 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>